<commit_message>
New Changes To xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/employee.xlsx
+++ b/src/main/resources/employee.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c2420ecdaa9d6e0/Desktop/java/Abhishek SQL/MavenPrac/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoges\IdeaProjects\ZorbaExamSubmission\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABDACC104841C9D9433C5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33D9C866-E91E-410D-9C16-65CC6EE1A15F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4051D60-19D1-494F-B5EC-B3CF95318E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="1240" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Employee_id</t>
-  </si>
-  <si>
-    <t>Emp_name</t>
-  </si>
-  <si>
-    <t>Emp_Salary</t>
-  </si>
-  <si>
-    <t>Emp_mobile</t>
-  </si>
-  <si>
-    <t>Emp_city</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>1004</t>
+  </si>
+  <si>
+    <t>1005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manager_id  </t>
+  </si>
+  <si>
+    <t>emp_dept</t>
+  </si>
+  <si>
+    <t>emp_share (%)</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20</t>
   </si>
 </sst>
 </file>
@@ -357,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -369,21 +402,164 @@
     <col min="2" max="2" width="32.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>